<commit_message>
begun implementing ROC curves for each prediction method in predict_recid
</commit_message>
<xml_diff>
--- a/2018_06_25 Data Element Dictionary.xlsx
+++ b/2018_06_25 Data Element Dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline Wang\OneDrive\Duke\Criminal Recidivism\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline Wang\OneDrive\Duke\Criminal Recidivism\psa-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{FC2BF87B-84E8-46F6-8F09-0A2CF348F98D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{53C24A3B-702E-41AC-A362-F5FAC6CCEFFB}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="8_{FC2BF87B-84E8-46F6-8F09-0A2CF348F98D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{089554BD-3C7B-4D35-A242-1A8952B04BA8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="7020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="352">
   <si>
     <t>InterviewId</t>
   </si>
@@ -1000,9 +1000,6 @@
   </si>
   <si>
     <t>Risk Assessment Question: Is the defendant’s current charge a Class A, B, or C Felony? (1=Yes, 0=No) Effective 1/1/2009 through 6/30/2013</t>
-  </si>
-  <si>
-    <t>RA1_New_Charge_While_Case_Pending</t>
   </si>
   <si>
     <t>Risk Assessment Question: Is the defendant charged with a new offense while there is a pending case? (1=Yes, 0=No) Effective 1/1/2009 through 6/30/2013</t>
@@ -1619,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1697,10 +1694,10 @@
     </row>
     <row r="13" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>351</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -1861,74 +1858,74 @@
     </row>
     <row r="34" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="B34" s="36" t="s">
         <v>325</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="B35" s="36" t="s">
         <v>327</v>
-      </c>
-      <c r="B35" s="36" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="B36" s="36" t="s">
         <v>329</v>
-      </c>
-      <c r="B36" s="36" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="B37" s="36" t="s">
         <v>331</v>
-      </c>
-      <c r="B37" s="36" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="B38" s="36" t="s">
         <v>333</v>
-      </c>
-      <c r="B38" s="36" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="34" t="s">
+        <v>334</v>
+      </c>
+      <c r="B39" s="36" t="s">
         <v>335</v>
-      </c>
-      <c r="B39" s="36" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="B40" s="36" t="s">
         <v>337</v>
-      </c>
-      <c r="B40" s="36" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="B41" s="36" t="s">
         <v>339</v>
-      </c>
-      <c r="B41" s="36" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="42" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="B42" s="36" t="s">
         <v>341</v>
-      </c>
-      <c r="B42" s="36" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="43" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -3185,19 +3182,19 @@
     </row>
     <row r="207" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A207" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B207" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="B207" s="5" t="s">
-        <v>344</v>
       </c>
       <c r="I207" s="5"/>
     </row>
     <row r="208" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A208" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="B208" s="5" t="s">
         <v>345</v>
-      </c>
-      <c r="B208" s="5" t="s">
-        <v>346</v>
       </c>
       <c r="I208" s="5"/>
     </row>
@@ -3456,10 +3453,10 @@
     </row>
     <row r="241" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A241" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B241" s="7" t="s">
         <v>349</v>
-      </c>
-      <c r="B241" s="7" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="242" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -3549,10 +3546,10 @@
     </row>
     <row r="254" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A254" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="B254" s="7" t="s">
         <v>347</v>
-      </c>
-      <c r="B254" s="7" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>